<commit_message>
a few more revisions
</commit_message>
<xml_diff>
--- a/tables/TableS6_global_results.xlsx
+++ b/tables/TableS6_global_results.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10420"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10913"/>
   <workbookPr date1904="1" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/cfree/Dropbox/Chris/UCSB/projects/nutrition/fortification/tables/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C043377D-B30C-E74E-B9BF-DA1D1F17304A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E38DADF0-1CB3-FB42-B068-D1DD89C09AF1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2040" yWindow="500" windowWidth="24040" windowHeight="20180" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1037,7 +1037,7 @@
   <dimension ref="A1:S23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="R22" sqref="R22"/>
+      <selection activeCell="K23" sqref="K23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2045,5 +2045,6 @@
     <sortCondition descending="1" ref="C4:C16"/>
   </sortState>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
</xml_diff>